<commit_message>
Changes done in code and added Base_page,Auto_Constant
</commit_message>
<xml_diff>
--- a/src/test/resources/DataDriven/LoginPage.xlsx
+++ b/src/test/resources/DataDriven/LoginPage.xlsx
@@ -4,34 +4,54 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14685" windowHeight="3600"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15675" windowHeight="6615"/>
   </bookViews>
   <sheets>
-    <sheet name="loginPage" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
-  <si>
-    <t>KAKBG0003</t>
-  </si>
-  <si>
-    <t>User_Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>objName</t>
+  </si>
+  <si>
+    <t>objPath</t>
+  </si>
+  <si>
+    <t>user_name</t>
+  </si>
+  <si>
+    <t>user_pwd</t>
+  </si>
+  <si>
+    <t>loginBtn</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>//a[@class='loginTop']</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>//span[normalize-space()='Login']</t>
+  </si>
+  <si>
+    <t>KAKBR0003</t>
   </si>
   <si>
     <t>Password@1</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>KAKBR0003</t>
   </si>
 </sst>
 </file>
@@ -47,12 +67,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color rgb="FF202124"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -63,7 +81,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -71,34 +89,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -398,51 +397,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Registration Test script added
</commit_message>
<xml_diff>
--- a/src/test/resources/DataDriven/LoginPage.xlsx
+++ b/src/test/resources/DataDriven/LoginPage.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Password</t>
   </si>
@@ -52,13 +52,28 @@
   </si>
   <si>
     <t>Password@1</t>
+  </si>
+  <si>
+    <t>Registration Details</t>
+  </si>
+  <si>
+    <t>Mobile No.</t>
+  </si>
+  <si>
+    <t>Email.ID</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>9423944227</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +86,14 @@
       <color rgb="FF202124"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -90,14 +113,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -397,15 +424,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
   </cols>
   <sheetData>
@@ -417,43 +444,68 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B11" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Applicant Details and Registration test scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/DataDriven/LoginPage.xlsx
+++ b/src/test/resources/DataDriven/LoginPage.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Password</t>
   </si>
@@ -67,13 +67,55 @@
   </si>
   <si>
     <t>9423944227</t>
+  </si>
+  <si>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>Applicant Name</t>
+  </si>
+  <si>
+    <t>PAN Card Number</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Present Address</t>
+  </si>
+  <si>
+    <t>Pincode</t>
+  </si>
+  <si>
+    <t>Permanent Address</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>HYBPL8765D</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>Mysore</t>
+  </si>
+  <si>
+    <t>2-06-2002</t>
+  </si>
+  <si>
+    <t>575322</t>
+  </si>
+  <si>
+    <t>560052</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +137,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -104,7 +160,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -112,16 +168,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -424,88 +501,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>3</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>5</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B20" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
'ScreenShot And Respective Change is RMI'
</commit_message>
<xml_diff>
--- a/src/test/resources/DataDriven/LoginPage.xlsx
+++ b/src/test/resources/DataDriven/LoginPage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15675" windowHeight="6615"/>
+    <workbookView xWindow="-60" yWindow="-105" windowWidth="15675" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>Email.ID</t>
   </si>
   <si>
-    <t>abc@gmail.com</t>
-  </si>
-  <si>
     <t>Form</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>9999999999</t>
+  </si>
+  <si>
+    <t>name31@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -504,7 +504,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,10 +542,10 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
         <v>30</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -554,7 +554,7 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
@@ -565,48 +565,48 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="G8" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="C9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="E9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Registration,OP,Email,Wallet Recharge,Services and test cases changes
</commit_message>
<xml_diff>
--- a/src/test/resources/DataDriven/LoginPage.xlsx
+++ b/src/test/resources/DataDriven/LoginPage.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-105" windowWidth="15675" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="12540" windowHeight="4110"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="69">
   <si>
     <t>Password</t>
   </si>
@@ -48,9 +48,6 @@
     <t>//span[normalize-space()='Login']</t>
   </si>
   <si>
-    <t>KAKBR0003</t>
-  </si>
-  <si>
     <t>Password@1</t>
   </si>
   <si>
@@ -84,12 +81,6 @@
     <t>Permanent Address</t>
   </si>
   <si>
-    <t>Ram</t>
-  </si>
-  <si>
-    <t>HYBPL8765D</t>
-  </si>
-  <si>
     <t>Bangalore</t>
   </si>
   <si>
@@ -102,13 +93,136 @@
     <t>560052</t>
   </si>
   <si>
-    <t>9999999999</t>
-  </si>
-  <si>
-    <t>name34@gmail.com</t>
-  </si>
-  <si>
     <t>02-Jun-2002</t>
+  </si>
+  <si>
+    <t>TVS</t>
+  </si>
+  <si>
+    <t>test tvs</t>
+  </si>
+  <si>
+    <t>9676545653</t>
+  </si>
+  <si>
+    <t>6452347865</t>
+  </si>
+  <si>
+    <t>Bengaluru</t>
+  </si>
+  <si>
+    <t>567456</t>
+  </si>
+  <si>
+    <t>Full name</t>
+  </si>
+  <si>
+    <t>Phone number</t>
+  </si>
+  <si>
+    <t>Mobile number</t>
+  </si>
+  <si>
+    <t>Address Line 1</t>
+  </si>
+  <si>
+    <t>KAKCB0003</t>
+  </si>
+  <si>
+    <t>OP Login</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>CMSOP</t>
+  </si>
+  <si>
+    <t>9738526155</t>
+  </si>
+  <si>
+    <t>Test Comment</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>sub1</t>
+  </si>
+  <si>
+    <t>sub2</t>
+  </si>
+  <si>
+    <t>ReachMyIndia Center Details</t>
+  </si>
+  <si>
+    <t>ReachMyIndia Application Approved</t>
+  </si>
+  <si>
+    <t>test@9vekviur.mailosaur.net</t>
+  </si>
+  <si>
+    <t>GonePassword@9</t>
+  </si>
+  <si>
+    <t>Wallet Amount</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>payu</t>
+  </si>
+  <si>
+    <t>KAKCB</t>
+  </si>
+  <si>
+    <t>Raj</t>
+  </si>
+  <si>
+    <t>HYBPL8765G</t>
+  </si>
+  <si>
+    <t>KAKC</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Invalid username</t>
+  </si>
+  <si>
+    <t>Invalid password</t>
+  </si>
+  <si>
+    <t>Invalid username/password</t>
+  </si>
+  <si>
+    <t>testuser@0g4tnuyv.mailosaur.net</t>
+  </si>
+  <si>
+    <t>testingteam508@gmail.com</t>
+  </si>
+  <si>
+    <t>Empty Amount</t>
+  </si>
+  <si>
+    <t>Less than 100</t>
+  </si>
+  <si>
+    <t>Amount with decimal</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>100.5</t>
   </si>
 </sst>
 </file>
@@ -187,7 +301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -198,6 +312,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -500,60 +630,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
@@ -562,131 +724,329 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="E9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="G9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>1</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B28" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>6</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>3</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B30" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>5</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B32" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E1" r:id="rId1"/>
+    <hyperlink ref="C16" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="A5" r:id="rId2"/>
+    <hyperlink ref="A6" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>